<commit_message>
Moved to correct location
</commit_message>
<xml_diff>
--- a/Assignment Instructions and framework/Gantt chart.xlsx
+++ b/Assignment Instructions and framework/Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25616"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25623"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfd74915eb265310/Teaching/1810ICT/Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD2D0859-CB59-4A9C-8932-A7E14286CF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D09D6DF-7B19-43F0-BE22-D9FE53B25D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Project Title</t>
   </si>
@@ -214,61 +214,16 @@
     <t>Stage 3 - Implementation</t>
   </si>
   <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
-  </si>
-  <si>
-    <t>Activity 27</t>
-  </si>
-  <si>
-    <t>Activity 28</t>
-  </si>
-  <si>
-    <t>Activity 29</t>
-  </si>
-  <si>
-    <t>Activity 30</t>
-  </si>
-  <si>
-    <t>Activity 31</t>
-  </si>
-  <si>
-    <t>Activity 32</t>
-  </si>
-  <si>
-    <t>Activity 33</t>
-  </si>
-  <si>
-    <t>Activity 34</t>
-  </si>
-  <si>
-    <t>Activity 35</t>
+    <t>Develop a testing plan</t>
+  </si>
+  <si>
+    <t>Develop a testing report</t>
+  </si>
+  <si>
+    <t>Create a user manual</t>
+  </si>
+  <si>
+    <t>Create a finalized data analysis report</t>
   </si>
 </sst>
 </file>
@@ -704,7 +659,572 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1084,14 +1604,14 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="37.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.125" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.75" style="1" bestFit="1" customWidth="1"/>
@@ -1407,465 +1927,705 @@
         <v>1</v>
       </c>
       <c r="D5" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="8">
         <v>0</v>
       </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1">
       <c r="B6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8">
         <v>0</v>
       </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1">
       <c r="B7" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="8">
         <v>0</v>
       </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1">
       <c r="B8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4</v>
+      </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8">
         <v>0</v>
       </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1">
       <c r="B9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>9</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="8">
         <v>0</v>
       </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1">
       <c r="B10" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>9</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="8">
         <v>0</v>
       </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="V10"/>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1">
       <c r="B11" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="7">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>3</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="8">
         <v>0</v>
       </c>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="V11"/>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1">
       <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>9</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="8">
         <v>0</v>
       </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1">
       <c r="B13" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="8">
         <v>0</v>
       </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1">
       <c r="B14" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="C14" s="7">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8">
         <v>0</v>
       </c>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1">
       <c r="B15" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="7"/>
+      <c r="C15" s="9">
+        <v>4</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8">
         <v>0</v>
       </c>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1">
       <c r="B16" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="C16" s="7">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7">
+        <v>2</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1">
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+    </row>
+    <row r="17" spans="2:29" ht="30" customHeight="1">
       <c r="B17" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="7">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7">
+        <v>2</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1">
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+    </row>
+    <row r="18" spans="2:29" ht="30" customHeight="1">
       <c r="B18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="C18" s="7">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1">
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+    </row>
+    <row r="19" spans="2:29" ht="30" customHeight="1">
       <c r="B19" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="C19" s="7">
+        <v>6</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1">
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+    </row>
+    <row r="20" spans="2:29" ht="30" customHeight="1">
       <c r="B20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="C20" s="7">
+        <v>10</v>
+      </c>
+      <c r="D20" s="7">
+        <v>13</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1">
-      <c r="B21" s="6" t="s">
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="17"/>
+      <c r="AA20" s="17"/>
+      <c r="AB20" s="17"/>
+      <c r="AC20" s="17"/>
+    </row>
+    <row r="21" spans="2:29" ht="30" customHeight="1">
+      <c r="B21" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="C21" s="7">
+        <v>10</v>
+      </c>
+      <c r="D21" s="7">
+        <v>4</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1">
-      <c r="B22" s="6" t="s">
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+    </row>
+    <row r="22" spans="2:29" ht="30" customHeight="1">
+      <c r="B22" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="C22" s="7">
+        <v>14</v>
+      </c>
+      <c r="D22" s="7">
+        <v>2</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1">
-      <c r="B23" s="6" t="s">
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+    </row>
+    <row r="23" spans="2:29" ht="30" customHeight="1">
+      <c r="B23" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="C23" s="7">
+        <v>14</v>
+      </c>
+      <c r="D23" s="7">
+        <v>5</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1">
-      <c r="B24" s="6" t="s">
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="17"/>
+      <c r="Y23" s="17"/>
+    </row>
+    <row r="24" spans="2:29" ht="30" customHeight="1">
+      <c r="B24" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="C24" s="7">
+        <v>18</v>
+      </c>
+      <c r="D24" s="7">
+        <v>5</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1">
-      <c r="B25" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="17"/>
+      <c r="AA24" s="17"/>
+      <c r="AB24" s="17"/>
+      <c r="AC24" s="17"/>
+    </row>
+    <row r="25" spans="2:29" ht="30" customHeight="1">
+      <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1">
-      <c r="B26" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="2:29" ht="30" customHeight="1">
+      <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1">
-      <c r="B27" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="2:29" ht="30" customHeight="1">
+      <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1">
-      <c r="B28" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="2:29" ht="30" customHeight="1">
+      <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1">
-      <c r="B29" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="2:29" ht="30" customHeight="1">
+      <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1">
-      <c r="B30" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="2:29" ht="30" customHeight="1">
+      <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
-      <c r="G30" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1">
-      <c r="B31" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="2:29" ht="30" customHeight="1">
+      <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1">
-      <c r="B32" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="2:29" ht="30" customHeight="1">
+      <c r="B32" s="6"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="8">
-        <v>0</v>
-      </c>
+      <c r="G32" s="8"/>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1">
-      <c r="B33" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="8">
-        <v>0</v>
-      </c>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1">
-      <c r="B34" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="8">
-        <v>0</v>
-      </c>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1">
-      <c r="B35" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="8">
-        <v>0</v>
-      </c>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1">
-      <c r="B36" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="8">
-        <v>0</v>
-      </c>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="2:7" ht="30" customHeight="1">
-      <c r="B37" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="B37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="8">
-        <v>0</v>
-      </c>
+      <c r="G37" s="8"/>
     </row>
     <row r="38" spans="2:7" ht="30" customHeight="1">
-      <c r="B38" s="6" t="s">
-        <v>48</v>
-      </c>
+      <c r="B38" s="6"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="8">
-        <v>0</v>
-      </c>
+      <c r="G38" s="8"/>
     </row>
     <row r="39" spans="2:7" ht="30" customHeight="1">
-      <c r="B39" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="B39" s="6"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
-      <c r="G39" s="8">
-        <v>0</v>
-      </c>
+      <c r="G39" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO39">
-    <cfRule type="expression" dxfId="8" priority="1">
+  <conditionalFormatting sqref="H25:BO39 K6:BO7 Q5:BO5 O8:BO8 H11 L11:BO11 Q12:BO12 J13:BO13 H14:J15 M14:BO15 H16:K17 N16:BO17 O18:BO18 H18:L19 Q19:BO19 Q9:BO10 AD20:BO20 H20:P21 U21:BO21 W22:BO22 H22:T23 H24:X24 Z23:BO23 AD24:BO24">
+    <cfRule type="expression" dxfId="48" priority="121">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="47" priority="123">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="46" priority="124">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="45" priority="125">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="44" priority="126">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="43" priority="127">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="11">
+    <cfRule type="expression" dxfId="42" priority="131">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="12">
+    <cfRule type="expression" dxfId="41" priority="132">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
+    <cfRule type="expression" dxfId="40" priority="128">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="expression" dxfId="39" priority="113">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="114">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="115">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="116">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="117">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="118">
+      <formula>J$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="119">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="120">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="expression" dxfId="31" priority="105">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="106">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="107">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="108">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="109">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="110">
+      <formula>J$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="111">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="112">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>N$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M8">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>M$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L8">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>L$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>H$4=period_selected</formula>
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
@@ -1874,7 +2634,7 @@
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2 H5:P5 H6:I7 I11:K11 H8:K10 H12:P12 H13:I13 K14:L15 L16:M17 M18:N18 M19:P19 L9:P10 Q20:AC20 Q21:T21 U22:V22 U23:Y23 Y24:AC24" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>

</xml_diff>